<commit_message>
Update spreadsheet to handle all current cases
</commit_message>
<xml_diff>
--- a/test_data/tracking-example.xlsx
+++ b/test_data/tracking-example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="prints" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="CT (porosity)" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Hardness (Vickers)" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="sem" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CT porosity" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Hardness Vickers" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,17 +22,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">SUBSYSTEM PARENT NAME</t>
+    <t xml:space="preserve">Parent</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature(c)</t>
   </si>
   <si>
+    <t xml:space="preserve">stress relief time (hr)</t>
+  </si>
+  <si>
     <t xml:space="preserve">wire composition</t>
   </si>
   <si>
@@ -45,9 +48,6 @@
     <t xml:space="preserve">stress relief temperature (°C)</t>
   </si>
   <si>
-    <t xml:space="preserve">CONDITION: stress relief time (hr)</t>
-  </si>
-  <si>
     <t xml:space="preserve">bead width (mm)</t>
   </si>
   <si>
@@ -99,13 +99,10 @@
     <t xml:space="preserve">M181210a</t>
   </si>
   <si>
-    <t xml:space="preserve">[1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 15, 14, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49, 50, 51, 52, 53, 54, 55, 56, 57, 58, 59, 60, 61, 62, 63, 64, 65, 66, 67, 68, 69, 70, 71, 72, 73, 74, 75, 76, 77, 79, 78, 80, 81, 82, 83, 84, 85, 86, 87, 88, 89, 90, 91, 92, 93, 94, 95, 96, 97, 98, 99, 100, 101, 102, 103, 104, 105, 106, 107, 108, 109, 110, 111, 112, 113, 114, 115, 116, 117, 118, 119, 120, 121, 122, 123, 124, 125]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[245128.7993, 245128.7993, 254556.83, 254556.83, 254556.83, 254556.83, 263984.8608, 263984.8608, 273412.8915, 273412.8915, 282840.9223, 282840.9223, 282840.9223, 292268.953, 292268.953, 311125.0145, 311125.0145, 339409.1067, 358265.1682, 358265.1682, 377121.2297, 377121.2297, 395977.2912, 414833.3527, 424261.3834, 424261.3834, 443117.4449, 452545.4756, 461973.5064, 471401.5371, 565681.8445, 575109.8753, 622250.029, 622250.029, 688246.2442, 716530.3364, 725958.3672, 801382.6131, 895662.9205, 942803.0742, 980515.1972, 1018227.32, 1027655.3509999999, 1055939.443, 1074795.505, 1093651.5659999999, 1112507.628, 1131363.689, 1150219.751, 1159647.781, 1253928.0890000002, 1282212.1809999999, 1338780.365, 1357636.427, 1357636.427, 1376492.4880000001, 1480200.8269999998, 1621621.2880000002, 1631049.3180000002, 1631049.3180000002, 1631049.3180000002, 1649905.38, 1715901.595, 1772469.78, 1791325.841, 1829037.9640000002, 1904462.21, 1951602.364, 1961030.394, 1970458.425, 2083594.794, 2093022.825, 2121306.917, 2140162.9790000003, 2168447.071, 2196731.163, 2215587.224, 2300439.501, 2300439.501, 2309867.5319999997, 2451287.9930000002, 2536140.27, 2592708.454, 2649276.639, 2696416.792, 2818981.192, 2950973.622, 2950973.622, 2960401.653, 3064109.9910000004, 3469515.313, 3705216.082, 3724072.143, 3818352.4510000004, 4016341.0960000004, 4044625.188, 4063481.25, 4129477.465, 4167189.588, 4252041.865, 4393462.326, 4412318.387, 4440602.48, 4553738.848999999, 4883719.925, 5458829.8, 5458829.8, 5798238.907000001, 5939659.368, 5967943.46, 6599621.52, 6646761.6729999995, 6675045.766, 7174731.395, 7212443.517999999, 7438716.256, 7532996.562999999, 7655560.9629999995, 7721557.177999999, 8409803.422, 8551223.883, 9984284.556, 10587678.52, 12001883.14, 13246383.19]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[77.64829165, 77.64829165, 78.63128577, 78.63128577, 78.63128577, 78.63128577, 79.59029841, 79.59029841, 80.52674077, 80.52674077, 81.44189571, 81.44189571, 81.44189571, 82.33693327, 82.33693327, 84.07084951, 84.07084951, 86.54492837, 88.11881632, 88.11881632, 89.63840489, 89.63840489, 91.10814816, 92.53194294, 93.22769796, 93.22769796, 94.58887827, 95.25501908, 95.91197101, 96.56004452, 102.6103588, 103.1772783, 105.922633, 105.922633, 109.5422716, 111.02275159999998, 111.50757320000001, 115.24279009999998, 119.59563370000001, 121.6580327, 123.25897990000001, 124.8193858, 125.20344779999999, 126.34172340000002, 127.089325, 127.82823300000001, 128.5586959, 129.28095090000002, 129.9952248, 130.34943700000002, 133.7903129, 134.78878500000002, 136.74251730000003, 137.3815103, 137.3815103, 138.0146138, 141.39715569999998, 145.763998, 146.0459407, 146.0459407, 146.0459407, 146.6065832, 148.53583840000002, 150.1504849, 150.6810564, 151.7311324, 153.7887543, 155.0473107, 155.2965833, 155.54505830000002, 158.4667729, 158.705428, 159.4171211, 159.8880754, 160.5893479, 161.2845485, 161.7447067, 163.78372009999998, 163.78372009999998, 164.0071634, 167.2881732, 169.1965679, 170.44529619999997, 171.6759908, 172.6882547, 175.26607140000002, 177.9599336, 177.9599336, 178.14925280000003, 180.2057217, 187.82644069999998, 191.9869191, 192.3120457, 193.9214264, 197.2168369, 197.67870469999997, 197.9854215, 199.05151740000002, 199.6556229, 201.0016565, 203.2057977, 203.4960921, 203.929987, 205.647373, 210.49932579999998, 218.457509, 218.457509, 222.8944019, 224.69201510000002, 225.04810440000003, 232.72344429999998, 233.27623369999998, 233.6066537, 239.2961299, 239.71466349999997, 242.195716, 243.21464139999998, 244.526613, 245.22726609999998, 252.3068689, 253.71329069999996, 267.160825, 272.43780630000003, 284.06447460000004, 293.5618149]</t>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
   </si>
   <si>
     <t xml:space="preserve">M181210a/GKN-7-21.125um-01.jpeg</t>
@@ -240,21 +237,22 @@
   </sheetPr>
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="10" style="0" width="8.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11"/>
   </cols>
@@ -269,7 +267,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -311,13 +309,16 @@
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>1.6</v>
+      <c r="D2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G2" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J2" s="0" t="n">
@@ -332,13 +333,16 @@
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>1.6</v>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G3" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J3" s="0" t="n">
@@ -353,13 +357,16 @@
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>1.6</v>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G4" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H4" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J4" s="0" t="n">
@@ -374,13 +381,16 @@
       <c r="C5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>1.6</v>
+      <c r="D5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G5" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H5" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J5" s="0" t="n">
@@ -395,13 +405,16 @@
       <c r="C6" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>1.6</v>
+      <c r="D6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G6" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H6" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -416,13 +429,16 @@
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1.6</v>
+      <c r="D7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G7" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J7" s="0" t="n">
@@ -437,13 +453,16 @@
       <c r="C8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>1.6</v>
+      <c r="D8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G8" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H8" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J8" s="0" t="n">
@@ -458,13 +477,16 @@
       <c r="C9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="0" t="n">
-        <v>1.6</v>
+      <c r="D9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G9" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H9" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J9" s="0" t="n">
@@ -479,13 +501,16 @@
       <c r="C10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="0" t="n">
-        <v>1.6</v>
+      <c r="D10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="G10" s="0" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="H10" s="0" t="n">
         <v>4.42</v>
       </c>
       <c r="J10" s="0" t="n">
@@ -512,7 +537,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,21 +552,22 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="ALS1" s="0"/>
       <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
       <c r="ALV1" s="0"/>
@@ -567,6 +593,9 @@
       <c r="B2" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="D2" s="0" t="s">
         <v>25</v>
       </c>
@@ -578,9 +607,6 @@
       </c>
       <c r="G2" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -601,8 +627,8 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -626,35 +652,35 @@
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for checking the parent and returning lists of errors from loading
</commit_message>
<xml_diff>
--- a/test_data/tracking-example.xlsx
+++ b/test_data/tracking-example.xlsx
@@ -96,7 +96,7 @@
     <t xml:space="preserve">FILE: porosity summary powerpoint</t>
   </si>
   <si>
-    <t xml:space="preserve">M181210a</t>
+    <t xml:space="preserve">sem</t>
   </si>
   <si>
     <t xml:space="preserve">a</t>
@@ -123,7 +123,7 @@
     <t xml:space="preserve">[0, 3.0, 6.0, 9.0, 12.0]</t>
   </si>
   <si>
-    <t xml:space="preserve">MH181210g</t>
+    <t xml:space="preserve">CT porosity</t>
   </si>
   <si>
     <t xml:space="preserve">[1, 2, 3, 4, 5]</t>
@@ -139,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -161,6 +161,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -205,13 +211,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -240,7 +250,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -323,7 +333,7 @@
       </c>
       <c r="J2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>124.65054365179</v>
+        <v>126.74471284316</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,7 +357,7 @@
       </c>
       <c r="J3" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>149.55460004379</v>
+        <v>115.801407221359</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -371,7 +381,7 @@
       </c>
       <c r="J4" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>124.21625333901</v>
+        <v>107.035496758743</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,7 +405,7 @@
       </c>
       <c r="J5" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>104.508117138451</v>
+        <v>110.337610377628</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,7 +429,7 @@
       </c>
       <c r="J6" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>116.66627297077</v>
+        <v>147.410744542474</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,7 +453,7 @@
       </c>
       <c r="J7" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>121.477052014529</v>
+        <v>136.951438356279</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,7 +477,7 @@
       </c>
       <c r="J8" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>135.044046613803</v>
+        <v>107.850190589054</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,7 +501,7 @@
       </c>
       <c r="J9" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>127.687728993932</v>
+        <v>146.694191922338</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,7 +525,7 @@
       </c>
       <c r="J10" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>114.144956094201</v>
+        <v>132.371137224924</v>
       </c>
     </row>
   </sheetData>
@@ -537,7 +547,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,11 +597,11 @@
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -628,7 +638,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -665,21 +675,21 @@
       <c r="D2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to turn cell values into json
</commit_message>
<xml_diff>
--- a/test_data/tracking-example.xlsx
+++ b/test_data/tracking-example.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -139,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -161,12 +161,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -220,7 +214,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -333,7 +327,7 @@
       </c>
       <c r="J2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>126.74471284316</v>
+        <v>141.180762625555</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +351,7 @@
       </c>
       <c r="J3" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>115.801407221359</v>
+        <v>103.42203963799</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,7 +375,7 @@
       </c>
       <c r="J4" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>107.035496758743</v>
+        <v>136.41731882861</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,7 +399,7 @@
       </c>
       <c r="J5" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>110.337610377628</v>
+        <v>121.496473531525</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,7 +423,7 @@
       </c>
       <c r="J6" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>147.410744542474</v>
+        <v>121.377084905406</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,7 +447,7 @@
       </c>
       <c r="J7" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>136.951438356279</v>
+        <v>138.634468187658</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,7 +471,7 @@
       </c>
       <c r="J8" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>107.850190589054</v>
+        <v>124.284117302677</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,7 +495,7 @@
       </c>
       <c r="J9" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>146.694191922338</v>
+        <v>133.75954971339</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,7 +519,7 @@
       </c>
       <c r="J10" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>132.371137224924</v>
+        <v>108.949986975698</v>
       </c>
     </row>
   </sheetData>
@@ -638,7 +632,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -669,9 +663,6 @@
       <c r="A2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="0" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Add keywords and remove blank column
</commit_message>
<xml_diff>
--- a/test_data/tracking-example.xlsx
+++ b/test_data/tracking-example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="sem" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,25 +30,25 @@
     <t xml:space="preserve">Parent</t>
   </si>
   <si>
-    <t xml:space="preserve">Temperature(c)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stress relief time (hr)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wire composition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wire diameter (mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wire density (g/cm^3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stress relief temperature (°C)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bead width (mm)</t>
+    <t xml:space="preserve">P:Temperature(c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p:stress relief time (hr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S:wire composition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S:wire diameter (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S:wire density (g/cm^3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P:stress relief temperature (°C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S:bead width (mm)</t>
   </si>
   <si>
     <t xml:space="preserve">G181030a</t>
@@ -81,13 +81,13 @@
     <t xml:space="preserve">G181030i</t>
   </si>
   <si>
-    <t xml:space="preserve">Label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Volume (µm^3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sphere Equivalent Diameter (µm)</t>
+    <t xml:space="preserve">P:Label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S:Volume (µm^3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S:Sphere Equivalent Diameter (µm)</t>
   </si>
   <si>
     <t xml:space="preserve">FILE: XCT surface</t>
@@ -111,7 +111,7 @@
     <t xml:space="preserve">M181210a/porosity summary.pptx</t>
   </si>
   <si>
-    <t xml:space="preserve">X-Distance (mm)</t>
+    <t xml:space="preserve">P:X-Distance (mm)</t>
   </si>
   <si>
     <t xml:space="preserve">MH181210a</t>
@@ -241,10 +241,10 @@
   </sheetPr>
   <dimension ref="A1:AMJ10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -253,12 +253,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="10" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="9" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="17" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="132" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -274,21 +275,22 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
       <c r="ALV1" s="0"/>
       <c r="ALW1" s="0"/>
@@ -316,18 +318,18 @@
       <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
+      <c r="E2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>141.180762625555</v>
+        <v>4.42</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>138.501278255577</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,18 +342,18 @@
       <c r="D3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>10</v>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>103.42203963799</v>
+        <v>4.42</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>120.419486305284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,18 +366,18 @@
       <c r="D4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>10</v>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>136.41731882861</v>
+        <v>4.42</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>128.813456802444</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,18 +390,18 @@
       <c r="D5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>10</v>
+      <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>121.496473531525</v>
+        <v>4.42</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>103.639050132966</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -412,18 +414,18 @@
       <c r="D6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F6" s="0" t="s">
-        <v>10</v>
+      <c r="E6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>121.377084905406</v>
+        <v>4.42</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>124.554042886406</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,18 +438,18 @@
       <c r="D7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="F7" s="0" t="s">
-        <v>10</v>
+      <c r="E7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>138.634468187658</v>
+        <v>4.42</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>145.267334924529</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,18 +462,18 @@
       <c r="D8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="F8" s="0" t="s">
-        <v>10</v>
+      <c r="E8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>124.284117302677</v>
+        <v>4.42</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>124.713089754236</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,18 +486,18 @@
       <c r="D9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>10</v>
+      <c r="E9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H9" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>133.75954971339</v>
+        <v>4.42</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>132.652372321217</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -508,18 +510,18 @@
       <c r="D10" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>10</v>
+      <c r="E10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>1.6</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>4.42</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <f aca="true">RAND()*50 + 100</f>
-        <v>108.949986975698</v>
+        <v>4.42</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <f aca="true">RAND()*50 + 100</f>
+        <v>125.092322445143</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +543,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -629,19 +631,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="5" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -651,11 +654,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -663,10 +665,10 @@
       <c r="A2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -677,10 +679,10 @@
       <c r="B3" s="0" t="s">
         <v>33</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update spreadsheet to include keywords
</commit_message>
<xml_diff>
--- a/test_data/tracking-example.xlsx
+++ b/test_data/tracking-example.xlsx
@@ -244,7 +244,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -329,7 +329,7 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>138.501278255577</v>
+        <v>145.925942779558</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,7 +353,7 @@
       </c>
       <c r="I3" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>120.419486305284</v>
+        <v>113.51426502216</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,7 +377,7 @@
       </c>
       <c r="I4" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>128.813456802444</v>
+        <v>129.808052176654</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,7 +401,7 @@
       </c>
       <c r="I5" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>103.639050132966</v>
+        <v>121.695171037026</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,7 +425,7 @@
       </c>
       <c r="I6" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>124.554042886406</v>
+        <v>106.569521109974</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,7 +449,7 @@
       </c>
       <c r="I7" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>145.267334924529</v>
+        <v>105.934298656101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,7 +473,7 @@
       </c>
       <c r="I8" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>124.713089754236</v>
+        <v>139.21842329569</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,7 +497,7 @@
       </c>
       <c r="I9" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>132.652372321217</v>
+        <v>114.559114039699</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,7 +521,7 @@
       </c>
       <c r="I10" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>125.092322445143</v>
+        <v>119.693396914127</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +543,7 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>